<commit_message>
2x excel update, 19 fertig
</commit_message>
<xml_diff>
--- a/feste-script/nublar_automation.xlsx
+++ b/feste-script/nublar_automation.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://concat-my.sharepoint.com/personal/oliver_antwerpen_concat_de/Documents/Kunden/ITSG/DiGeN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21663F41-B11C-4F3E-853A-E29AB1E541B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B19A0ED-5AFF-485E-AD1B-FB3F758D4CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6FC2A35C-60ED-4314-86AB-AEC6FD6F7C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$O$36</definedName>
+  </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="88">
-  <si>
-    <t>FeSte</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="91">
   <si>
     <t>#</t>
   </si>
@@ -102,6 +102,18 @@
     <t>Rename Enclosures</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Rename Server Hardware Types</t>
+  </si>
+  <si>
+    <t>FS: template+rename</t>
+  </si>
+  <si>
     <t>Configure NTP</t>
   </si>
   <si>
@@ -111,12 +123,6 @@
     <t>X_01_ntp.yml</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>ov-timelocal.yml</t>
   </si>
   <si>
@@ -279,16 +285,22 @@
     <t>Add Hypervisor Manager</t>
   </si>
   <si>
+    <t>X_03_addhypervisormanager.yml</t>
+  </si>
+  <si>
+    <t>/rest/hypervisor-managers</t>
+  </si>
+  <si>
+    <t>Add Hypervisor Cluster Profiles</t>
+  </si>
+  <si>
+    <t>Add Hypervisors</t>
+  </si>
+  <si>
+    <t>Create SP Template</t>
+  </si>
+  <si>
     <t>OlAnt</t>
-  </si>
-  <si>
-    <t>Add Hypervisor Cluster Profiles</t>
-  </si>
-  <si>
-    <t>Add Hypervisors</t>
-  </si>
-  <si>
-    <t>Create SP Template</t>
   </si>
   <si>
     <t>12,13,14</t>
@@ -339,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -411,12 +423,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -461,16 +486,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -785,19 +813,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C3E72-56EF-455D-9F96-4919901547B8}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.140625" style="16" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" style="16" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -805,176 +833,197 @@
     <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="40.7109375" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="58.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15">
-      <c r="A1" s="18"/>
-      <c r="J1" s="19" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="19"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-    </row>
-    <row r="2" spans="1:15" ht="15">
-      <c r="A2" s="18" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="J2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" t="s">
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="19"/>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="15">
-      <c r="A3" s="18"/>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="J3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="18"/>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="12" t="s">
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="19"/>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15">
-      <c r="A4" s="18"/>
-      <c r="B4" t="s">
+      <c r="C4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="19">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-    </row>
-    <row r="5" spans="1:15" ht="15">
-      <c r="A5" s="18"/>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-    </row>
-    <row r="6" spans="1:15" ht="15">
-      <c r="A6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-    </row>
-    <row r="7" spans="1:15" ht="15">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="J5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="19">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="6">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>27</v>
+      <c r="J7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>23</v>
       </c>
       <c r="M7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -985,14 +1034,14 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:15" ht="15">
+    <row r="9" spans="1:15">
       <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -1003,14 +1052,14 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:15" ht="15">
+    <row r="10" spans="1:15">
       <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -1021,14 +1070,14 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:15" ht="15">
+    <row r="11" spans="1:15">
       <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -1039,20 +1088,20 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:15" ht="15">
+    <row r="12" spans="1:15">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="14"/>
@@ -1061,597 +1110,611 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:15" ht="15">
+    <row r="13" spans="1:15">
       <c r="A13" s="7">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="7">
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I14" s="14"/>
       <c r="J14" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="8">
         <v>4</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15">
-      <c r="A16" s="18">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="19">
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+        <v>44</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15">
-      <c r="A17" s="18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="19">
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15">
-      <c r="A18" s="18">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="19">
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18" t="s">
         <v>50</v>
       </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="H18" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
       <c r="M18" t="s">
-        <v>53</v>
-      </c>
-      <c r="O18" s="20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="15">
-      <c r="A19" s="18"/>
+      <c r="O18" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="19"/>
       <c r="B19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+        <v>56</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:15" ht="15">
-      <c r="A20" s="18"/>
+    <row r="20" spans="1:15">
+      <c r="A20" s="19"/>
       <c r="B20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+        <v>57</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:15" ht="15">
-      <c r="A21" s="18">
+    <row r="21" spans="1:15">
+      <c r="A21" s="19">
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+        <v>58</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
       <c r="H21" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="15">
-      <c r="A22" s="18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="19">
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+        <v>61</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
       <c r="H22" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15">
-      <c r="A23" s="18">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="19">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+        <v>64</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
       <c r="H23" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="15">
-      <c r="A24" s="18">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="19">
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
       <c r="H24" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15">
-      <c r="A25" s="18">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="19">
         <v>13</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
       <c r="H25" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N25">
         <v>12</v>
       </c>
       <c r="O25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="15">
-      <c r="A26" s="18">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="19">
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+        <v>74</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
       <c r="H26" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N26">
         <v>12</v>
       </c>
       <c r="O26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="15">
-      <c r="A27" s="18">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="19">
         <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+        <v>78</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
       <c r="H27" s="16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="15">
-      <c r="A28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-    </row>
-    <row r="29" spans="1:15" ht="15">
-      <c r="A29" s="18">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="19">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="I29" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-    </row>
-    <row r="30" spans="1:15" ht="15">
-      <c r="A30" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="19">
+        <v>18</v>
+      </c>
       <c r="B30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+        <v>85</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:15" ht="15">
-      <c r="A31" s="18"/>
+    <row r="31" spans="1:15">
+      <c r="A31" s="19"/>
       <c r="B31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+        <v>86</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:15" ht="15">
-      <c r="A32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-    </row>
-    <row r="33" spans="1:15" ht="15">
-      <c r="A33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-    </row>
-    <row r="34" spans="1:15" ht="15">
-      <c r="A34" s="18">
-        <v>16</v>
+    <row r="32" spans="1:15">
+      <c r="A32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="19">
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+        <v>87</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
       <c r="I34" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="J34" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="N34" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="O34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="15">
-      <c r="A35" s="18"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="19"/>
       <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="39" spans="1:15" ht="15">
-      <c r="A39" s="18"/>
+        <v>90</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="19"/>
       <c r="M39" s="17"/>
     </row>
-    <row r="40" spans="1:15" ht="15">
-      <c r="A40" s="18"/>
+    <row r="40" spans="1:15">
+      <c r="A40" s="19"/>
       <c r="M40" s="17"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:O36" xr:uid="{75D72059-CA16-47AB-B54F-E480A496FC04}"/>
   <mergeCells count="1">
     <mergeCell ref="J1:L1"/>
   </mergeCells>
@@ -1872,6 +1935,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1880,20 +1949,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7949D86A-4ECE-4ACB-803E-DBA0DC1FCA2F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9413D6E-CC83-4DA9-B04D-98395BEF15B5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A004C57-C4A2-4105-A373-B1C1CD783209}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A004C57-C4A2-4105-A373-B1C1CD783209}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9413D6E-CC83-4DA9-B04D-98395BEF15B5}"/>
 </file>
</xml_diff>

<commit_message>
api anmeldung in eigene funktion
</commit_message>
<xml_diff>
--- a/feste-script/nublar_automation.xlsx
+++ b/feste-script/nublar_automation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://concat-my.sharepoint.com/personal/oliver_antwerpen_concat_de/Documents/Kunden/ITSG/DiGeN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B19A0ED-5AFF-485E-AD1B-FB3F758D4CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FBD5AF3-2F4D-46A7-973C-99A1FD44FA9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6FC2A35C-60ED-4314-86AB-AEC6FD6F7C27}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="90">
   <si>
     <t>#</t>
   </si>
@@ -48,30 +48,30 @@
     <t>Ansible</t>
   </si>
   <si>
-    <t>Param. geliefert</t>
-  </si>
-  <si>
-    <t>Param. in Excel</t>
+    <t>Para geliefert</t>
+  </si>
+  <si>
+    <t>Para in Excel</t>
   </si>
   <si>
     <t>Fertig</t>
   </si>
   <si>
+    <t>Zuständig</t>
+  </si>
+  <si>
+    <t>informiert</t>
+  </si>
+  <si>
+    <t>umgesetzt</t>
+  </si>
+  <si>
+    <t>verifiziert</t>
+  </si>
+  <si>
     <t>Filename</t>
   </si>
   <si>
-    <t>Zuständigkeit</t>
-  </si>
-  <si>
-    <t>informiert</t>
-  </si>
-  <si>
-    <t>umgesetzt</t>
-  </si>
-  <si>
-    <t>erfolgreich getestet</t>
-  </si>
-  <si>
     <t>basierend auf Template</t>
   </si>
   <si>
@@ -87,15 +87,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>=OlAnt geliefert</t>
-  </si>
-  <si>
-    <t>=FeSte geliefert</t>
-  </si>
-  <si>
-    <t>=OK von OlAnt</t>
-  </si>
-  <si>
     <t>Configure Certificate</t>
   </si>
   <si>
@@ -108,10 +99,19 @@
     <t>?</t>
   </si>
   <si>
+    <t>X_19_renameenclosures.yml</t>
+  </si>
+  <si>
+    <t>oneview_enclosure</t>
+  </si>
+  <si>
     <t>Rename Server Hardware Types</t>
   </si>
   <si>
-    <t>FS: template+rename</t>
+    <t>X_16_renameserverhardwaretypes.yml</t>
+  </si>
+  <si>
+    <t>oneview_server_hardware_type</t>
   </si>
   <si>
     <t>Configure NTP</t>
@@ -189,15 +189,12 @@
     <t>Add Storage System &amp; Pool</t>
   </si>
   <si>
-    <t>Ticket in Github erstellt</t>
+    <t>Ticket in Github oder REST-API</t>
   </si>
   <si>
     <t>X_10_storagesystem.yml</t>
   </si>
   <si>
-    <t>HP?</t>
-  </si>
-  <si>
     <t>ov-storagesystem.yml</t>
   </si>
   <si>
@@ -294,13 +291,13 @@
     <t>Add Hypervisor Cluster Profiles</t>
   </si>
   <si>
+    <t>OlAnt</t>
+  </si>
+  <si>
     <t>Add Hypervisors</t>
   </si>
   <si>
     <t>Create SP Template</t>
-  </si>
-  <si>
-    <t>OlAnt</t>
   </si>
   <si>
     <t>12,13,14</t>
@@ -351,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -436,12 +433,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -479,9 +509,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -494,6 +521,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -814,36 +851,36 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.140625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="16" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="15" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="38.42578125" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
     <col min="15" max="15" width="58.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="19"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="19" t="s">
+    <row r="1" spans="1:15" ht="15">
+      <c r="A1" s="18"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+    </row>
+    <row r="2" spans="1:15" ht="15">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -864,19 +901,19 @@
       <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="15" t="s">
         <v>11</v>
       </c>
       <c r="M2" t="s">
@@ -889,97 +926,109 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="19"/>
+    <row r="3" spans="1:15" ht="15">
+      <c r="A3" s="18"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="19"/>
-      <c r="J3" s="12" t="s">
+      <c r="C3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="15"/>
+    </row>
+    <row r="4" spans="1:15" ht="15">
+      <c r="A4" s="18"/>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="C4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:15" ht="15">
+      <c r="A5" s="18">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="19"/>
-      <c r="B4" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="I5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="19">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="L5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="J5" s="5" t="s">
+      <c r="M5" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:15" ht="15">
+      <c r="A6" s="18">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="19">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="I6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19" t="s">
+      <c r="M6" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:15" ht="15">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -999,24 +1048,24 @@
       <c r="G7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="14"/>
+      <c r="I7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="14" t="s">
         <v>28</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>23</v>
       </c>
       <c r="M7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="15">
       <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>30</v>
@@ -1029,12 +1078,12 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="K8" s="23"/>
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" spans="1:15" ht="15">
       <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
         <v>31</v>
@@ -1047,12 +1096,12 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="K9" s="23"/>
+      <c r="L9" s="14"/>
+    </row>
+    <row r="10" spans="1:15" ht="15">
       <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
         <v>32</v>
@@ -1065,12 +1114,12 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="K10" s="23"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" ht="15">
       <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
         <v>33</v>
@@ -1083,12 +1132,12 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="K11" s="23"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:15" ht="15">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
         <v>34</v>
@@ -1105,12 +1154,12 @@
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="K12" s="23"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:15" ht="15">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -1128,24 +1177,24 @@
         <v>16</v>
       </c>
       <c r="G13" s="10"/>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="14"/>
+      <c r="I13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="M13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" ht="15">
       <c r="A14" s="7">
         <v>2</v>
       </c>
@@ -1165,24 +1214,24 @@
       <c r="G14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="14"/>
+      <c r="I14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="M14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" ht="15">
       <c r="A15" s="8">
         <v>4</v>
       </c>
@@ -1200,518 +1249,513 @@
         <v>16</v>
       </c>
       <c r="G15" s="11"/>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="14"/>
+      <c r="I15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="M15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="19">
+    <row r="16" spans="1:15" ht="15">
+      <c r="A16" s="18">
         <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="16" t="s">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="I16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="M16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="19">
+    <row r="17" spans="1:15" ht="15">
+      <c r="A17" s="18">
         <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="16" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="I17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="M17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="19">
+    <row r="18" spans="1:15" ht="15">
+      <c r="A18" s="18">
         <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19" t="s">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="I18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="M18" t="s">
         <v>53</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" t="s">
+      <c r="O18" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="O18" s="18" t="s">
+    </row>
+    <row r="19" spans="1:15" ht="15">
+      <c r="A19" s="18"/>
+      <c r="B19" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="19"/>
-      <c r="B19" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="14"/>
+    </row>
+    <row r="20" spans="1:15" ht="15">
+      <c r="A20" s="18"/>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="19"/>
-      <c r="B20" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="14"/>
+    </row>
+    <row r="21" spans="1:15" ht="15">
+      <c r="A21" s="18">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="19">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="I21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="16" t="s">
+      <c r="M21" t="s">
         <v>59</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M21" t="s">
+    </row>
+    <row r="22" spans="1:15" ht="15">
+      <c r="A22" s="18">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="A22" s="19">
-        <v>8</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="I22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="16" t="s">
+      <c r="M22" t="s">
         <v>62</v>
       </c>
-      <c r="J22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M22" t="s">
+    </row>
+    <row r="23" spans="1:15" ht="15">
+      <c r="A23" s="18">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="19">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="I23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="16" t="s">
+      <c r="M23" t="s">
         <v>65</v>
       </c>
-      <c r="J23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M23" t="s">
+    </row>
+    <row r="24" spans="1:15" ht="15">
+      <c r="A24" s="18">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="19">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="I24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="16" t="s">
+      <c r="M24" t="s">
         <v>68</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M24" t="s">
+    </row>
+    <row r="25" spans="1:15" ht="15">
+      <c r="A25" s="18">
+        <v>13</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="19">
-        <v>13</v>
-      </c>
-      <c r="B25" s="17" t="s">
+      <c r="C25" s="18"/>
+      <c r="D25" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="I25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="16" t="s">
+      <c r="M25" t="s">
         <v>71</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M25" t="s">
-        <v>72</v>
       </c>
       <c r="N25">
         <v>12</v>
       </c>
       <c r="O25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15">
+      <c r="A26" s="18">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="19">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C26" s="18"/>
+      <c r="D26" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="I26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="16" t="s">
+      <c r="M26" t="s">
         <v>75</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M26" t="s">
-        <v>76</v>
       </c>
       <c r="N26">
         <v>12</v>
       </c>
       <c r="O26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15">
+      <c r="A27" s="21">
+        <v>15</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="19">
-        <v>15</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C27" s="21"/>
+      <c r="D27" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="I27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="16" t="s">
+      <c r="M27" t="s">
         <v>79</v>
       </c>
-      <c r="J27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="N27">
+        <v>12</v>
+      </c>
+      <c r="O27" t="s">
         <v>80</v>
       </c>
-      <c r="O27" t="s">
+    </row>
+    <row r="28" spans="1:15" ht="15">
+      <c r="A28" s="18">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="19">
-        <v>3</v>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="I28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="M28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15">
+      <c r="A29" s="18">
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M29" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="A30" s="19">
-        <v>18</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C29" s="18"/>
+      <c r="D29" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="14"/>
+    </row>
+    <row r="30" spans="1:15" ht="15">
+      <c r="A30" s="21"/>
+      <c r="B30" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="19"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="14"/>
+    </row>
+    <row r="31" spans="1:15" ht="15">
+      <c r="A31" s="18">
+        <v>17</v>
+      </c>
       <c r="B31" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+        <v>87</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="19">
-        <v>17</v>
-      </c>
-      <c r="B34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="I34" s="16" t="s">
+      <c r="K31" s="23"/>
+      <c r="L31" s="14"/>
+      <c r="N31" t="s">
         <v>88</v>
       </c>
-      <c r="J34" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="N34" t="s">
+      <c r="O31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15">
+      <c r="A32" s="18"/>
+      <c r="B32" t="s">
         <v>89</v>
       </c>
-      <c r="O34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="19"/>
-      <c r="B35" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="A39" s="19"/>
-      <c r="M39" s="17"/>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="A40" s="19"/>
-      <c r="M40" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="1:13" ht="15">
+      <c r="A33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+    </row>
+    <row r="34" spans="1:13" ht="15">
+      <c r="A34" s="18"/>
+    </row>
+    <row r="35" spans="1:13" ht="15">
+      <c r="A35" s="18"/>
+    </row>
+    <row r="36" spans="1:13" ht="15">
+      <c r="A36" s="18"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="18"/>
+      <c r="M39" s="16"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="18"/>
+      <c r="M40" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:O36" xr:uid="{75D72059-CA16-47AB-B54F-E480A496FC04}"/>

</xml_diff>

<commit_message>
10 screenshot, 2x excel update, 17 angefangen ,18 angefangen
</commit_message>
<xml_diff>
--- a/feste-script/nublar_automation.xlsx
+++ b/feste-script/nublar_automation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_e60\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_879\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C06D5D5A-01AF-49CB-B593-5A758A6CBDAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2921C89F-0D50-4FC5-ACE5-8F881B30EA95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{6FC2A35C-60ED-4314-86AB-AEC6FD6F7C27}"/>
   </bookViews>
@@ -480,13 +480,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -808,7 +808,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -831,13 +831,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15">
-      <c r="A1" s="18"/>
+      <c r="A1" s="20"/>
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
       <c r="L1" s="21"/>
     </row>
     <row r="2" spans="1:15" ht="15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -861,13 +861,13 @@
       <c r="H2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="20" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="15" t="s">
@@ -884,61 +884,61 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15">
-      <c r="A3" s="18"/>
+      <c r="A3" s="20"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="18"/>
+      <c r="C3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="20"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:15" ht="15">
-      <c r="A4" s="18"/>
+      <c r="A4" s="20"/>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
+      <c r="C4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
       <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:15" ht="15">
-      <c r="A5" s="18">
+      <c r="A5" s="20">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="18"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="20"/>
       <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
@@ -956,19 +956,19 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A6" s="18">
+      <c r="A6" s="20">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
@@ -1224,19 +1224,19 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15">
-      <c r="A16" s="18">
+      <c r="A16" s="20">
         <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
       <c r="I16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1254,19 +1254,19 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="15">
-      <c r="A17" s="18">
+      <c r="A17" s="20">
         <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
       <c r="I17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1284,19 +1284,19 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="15">
-      <c r="A18" s="18">
+      <c r="A18" s="20">
         <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20" t="s">
         <v>51</v>
       </c>
       <c r="H18" s="15" t="s">
@@ -1318,19 +1318,19 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="15">
-      <c r="A19" s="18">
+      <c r="A19" s="20">
         <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="15" t="s">
         <v>52</v>
       </c>
@@ -1340,19 +1340,19 @@
       <c r="L19" s="14"/>
     </row>
     <row r="20" spans="1:15" ht="15">
-      <c r="A20" s="18">
+      <c r="A20" s="20">
         <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="15" t="s">
         <v>52</v>
       </c>
@@ -1362,19 +1362,19 @@
       <c r="L20" s="14"/>
     </row>
     <row r="21" spans="1:15" ht="15">
-      <c r="A21" s="18">
+      <c r="A21" s="20">
         <v>7</v>
       </c>
       <c r="B21" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
       <c r="I21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1392,19 +1392,19 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="15">
-      <c r="A22" s="18">
+      <c r="A22" s="20">
         <v>8</v>
       </c>
       <c r="B22" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
       <c r="I22" s="5" t="s">
         <v>19</v>
       </c>
@@ -1422,19 +1422,19 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="15">
-      <c r="A23" s="18">
+      <c r="A23" s="20">
         <v>9</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="5" t="s">
         <v>19</v>
       </c>
@@ -1452,19 +1452,19 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="15">
-      <c r="A24" s="18">
+      <c r="A24" s="20">
         <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
       <c r="I24" s="5" t="s">
         <v>19</v>
       </c>
@@ -1482,19 +1482,19 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="15">
-      <c r="A25" s="18">
+      <c r="A25" s="20">
         <v>13</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
       <c r="I25" s="5" t="s">
         <v>19</v>
       </c>
@@ -1518,19 +1518,19 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="15">
-      <c r="A26" s="18">
+      <c r="A26" s="20">
         <v>14</v>
       </c>
       <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
       <c r="I26" s="5" t="s">
         <v>19</v>
       </c>
@@ -1554,19 +1554,19 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A27" s="19">
+      <c r="A27" s="18">
         <v>15</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
       <c r="I27" s="5" t="s">
         <v>19</v>
       </c>
@@ -1590,19 +1590,19 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="15">
-      <c r="A28" s="18">
+      <c r="A28" s="20">
         <v>3</v>
       </c>
       <c r="B28" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
       <c r="I28" s="5" t="s">
         <v>19</v>
       </c>
@@ -1620,19 +1620,19 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="15">
-      <c r="A29" s="18">
+      <c r="A29" s="20">
         <v>18</v>
       </c>
       <c r="B29" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="15" t="s">
         <v>86</v>
       </c>
@@ -1642,36 +1642,36 @@
       <c r="L29" s="14"/>
     </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A30" s="19"/>
-      <c r="B30" s="20" t="s">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="14"/>
     </row>
     <row r="31" spans="1:15" ht="15">
-      <c r="A31" s="18">
+      <c r="A31" s="20">
         <v>17</v>
       </c>
       <c r="B31" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
       <c r="H31" s="15" t="s">
         <v>52</v>
       </c>
@@ -1693,42 +1693,42 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="15">
-      <c r="A32" s="18"/>
+      <c r="A32" s="20"/>
       <c r="B32" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
     </row>
     <row r="33" spans="1:13" ht="15">
-      <c r="A33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
+      <c r="A33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
     </row>
     <row r="34" spans="1:13" ht="15">
-      <c r="A34" s="18"/>
+      <c r="A34" s="20"/>
     </row>
     <row r="35" spans="1:13" ht="15">
-      <c r="A35" s="18"/>
+      <c r="A35" s="20"/>
     </row>
     <row r="36" spans="1:13" ht="15">
-      <c r="A36" s="18"/>
+      <c r="A36" s="20"/>
     </row>
     <row r="39" spans="1:13" ht="15">
-      <c r="A39" s="18"/>
+      <c r="A39" s="20"/>
       <c r="M39" s="16"/>
     </row>
     <row r="40" spans="1:13" ht="15">
-      <c r="A40" s="18"/>
+      <c r="A40" s="20"/>
       <c r="M40" s="16"/>
     </row>
   </sheetData>
@@ -1744,9 +1744,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1959,16 +1962,13 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A004C57-C4A2-4105-A373-B1C1CD783209}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9413D6E-CC83-4DA9-B04D-98395BEF15B5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1976,5 +1976,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9413D6E-CC83-4DA9-B04D-98395BEF15B5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A004C57-C4A2-4105-A373-B1C1CD783209}"/>
 </file>
</xml_diff>

<commit_message>
10 zu 90prozent fertig
</commit_message>
<xml_diff>
--- a/feste-script/nublar_automation.xlsx
+++ b/feste-script/nublar_automation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_879\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://concat-my.sharepoint.com/personal/oliver_antwerpen_concat_de/Documents/Kunden/ITSG/DiGeN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2921C89F-0D50-4FC5-ACE5-8F881B30EA95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5D6BA0E-293F-4D4E-B02F-8BCBDE72E963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{6FC2A35C-60ED-4314-86AB-AEC6FD6F7C27}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6FC2A35C-60ED-4314-86AB-AEC6FD6F7C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="90">
   <si>
     <t>#</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>X_10_storagesystem.yml</t>
-  </si>
-  <si>
-    <t>ov-storagesystem.yml</t>
   </si>
   <si>
     <t>https://github.com/HewlettPackard/oneview-ansible/issues/456</t>
@@ -480,13 +477,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -807,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C3E72-56EF-455D-9F96-4919901547B8}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -830,14 +827,14 @@
     <col min="15" max="15" width="58.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15">
-      <c r="A1" s="20"/>
+    <row r="1" spans="1:15">
+      <c r="A1" s="18"/>
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:15" ht="15">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -861,13 +858,13 @@
       <c r="H2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="18" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="15" t="s">
@@ -883,62 +880,62 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15">
-      <c r="A3" s="20"/>
+    <row r="3" spans="1:15">
+      <c r="A3" s="18"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="20"/>
+      <c r="C3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="18"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:15" ht="15">
-      <c r="A4" s="20"/>
+    <row r="4" spans="1:15">
+      <c r="A4" s="18"/>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="C4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:15" ht="15">
-      <c r="A5" s="20">
+    <row r="5" spans="1:15">
+      <c r="A5" s="18">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="20"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="18"/>
       <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
@@ -955,20 +952,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A6" s="20">
+    <row r="6" spans="1:15" ht="15" thickBot="1">
+      <c r="A6" s="18">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
@@ -985,7 +982,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15">
+    <row r="7" spans="1:15">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -1022,7 +1019,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15">
+    <row r="8" spans="1:15">
       <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>30</v>
@@ -1040,7 +1037,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="14"/>
     </row>
-    <row r="9" spans="1:15" ht="15">
+    <row r="9" spans="1:15">
       <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
         <v>31</v>
@@ -1058,7 +1055,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="1:15" ht="15">
+    <row r="10" spans="1:15">
       <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
         <v>32</v>
@@ -1076,7 +1073,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:15" ht="15">
+    <row r="11" spans="1:15">
       <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
         <v>33</v>
@@ -1094,7 +1091,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="14"/>
     </row>
-    <row r="12" spans="1:15" ht="15">
+    <row r="12" spans="1:15">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
         <v>34</v>
@@ -1116,7 +1113,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:15" ht="15">
+    <row r="13" spans="1:15">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -1151,7 +1148,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15">
+    <row r="14" spans="1:15">
       <c r="A14" s="7">
         <v>2</v>
       </c>
@@ -1188,7 +1185,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1">
+    <row r="15" spans="1:15" ht="15" thickBot="1">
       <c r="A15" s="8">
         <v>4</v>
       </c>
@@ -1223,20 +1220,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15">
-      <c r="A16" s="20">
+    <row r="16" spans="1:15">
+      <c r="A16" s="18">
         <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="I16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1253,20 +1250,20 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15">
-      <c r="A17" s="20">
+    <row r="17" spans="1:15">
+      <c r="A17" s="18">
         <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
       <c r="I17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1283,20 +1280,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15">
-      <c r="A18" s="20">
+    <row r="18" spans="1:15">
+      <c r="A18" s="18">
         <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20" t="s">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18" t="s">
         <v>51</v>
       </c>
       <c r="H18" s="15" t="s">
@@ -1310,27 +1307,24 @@
       <c r="L18" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="M18" t="s">
+      <c r="O18" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="O18" s="17" t="s">
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="18">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="15">
-      <c r="A19" s="20">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="15" t="s">
         <v>52</v>
       </c>
@@ -1339,20 +1333,20 @@
       <c r="K19" s="5"/>
       <c r="L19" s="14"/>
     </row>
-    <row r="20" spans="1:15" ht="15">
-      <c r="A20" s="20">
+    <row r="20" spans="1:15">
+      <c r="A20" s="18">
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
+        <v>56</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="15" t="s">
         <v>52</v>
       </c>
@@ -1361,248 +1355,248 @@
       <c r="K20" s="5"/>
       <c r="L20" s="14"/>
     </row>
-    <row r="21" spans="1:15" ht="15">
-      <c r="A21" s="20">
+    <row r="21" spans="1:15">
+      <c r="A21" s="18">
         <v>7</v>
       </c>
       <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="I21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="I21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21" s="14" t="s">
+      <c r="M21" t="s">
         <v>59</v>
       </c>
-      <c r="M21" t="s">
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="18">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" ht="15">
-      <c r="A22" s="20">
-        <v>8</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="I22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="I22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="14" t="s">
+      <c r="M22" t="s">
         <v>62</v>
       </c>
-      <c r="M22" t="s">
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="18">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" ht="15">
-      <c r="A23" s="20">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="I23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="I23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" s="14" t="s">
+      <c r="M23" t="s">
         <v>65</v>
       </c>
-      <c r="M23" t="s">
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="18">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" ht="15">
-      <c r="A24" s="20">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="I24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="I24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L24" s="14" t="s">
+      <c r="M24" t="s">
         <v>68</v>
       </c>
-      <c r="M24" t="s">
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="18">
+        <v>13</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" ht="15">
-      <c r="A25" s="20">
-        <v>13</v>
-      </c>
-      <c r="B25" s="16" t="s">
+      <c r="C25" s="18"/>
+      <c r="D25" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="I25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="I25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L25" s="14" t="s">
+      <c r="M25" t="s">
         <v>71</v>
-      </c>
-      <c r="M25" t="s">
-        <v>72</v>
       </c>
       <c r="N25">
         <v>12</v>
       </c>
       <c r="O25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="18">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" ht="15">
-      <c r="A26" s="20">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C26" s="18"/>
+      <c r="D26" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="I26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="I26" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" s="14" t="s">
+      <c r="M26" t="s">
         <v>75</v>
-      </c>
-      <c r="M26" t="s">
-        <v>76</v>
       </c>
       <c r="N26">
         <v>12</v>
       </c>
       <c r="O26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickBot="1">
+      <c r="A27" s="19">
+        <v>15</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A27" s="18">
-        <v>15</v>
-      </c>
-      <c r="B27" s="19" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="I27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="I27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L27" s="14" t="s">
+      <c r="M27" t="s">
         <v>79</v>
-      </c>
-      <c r="M27" t="s">
-        <v>80</v>
       </c>
       <c r="N27">
         <v>12</v>
       </c>
       <c r="O27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="18">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" ht="15">
-      <c r="A28" s="20">
-        <v>3</v>
-      </c>
-      <c r="B28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="I28" s="5" t="s">
         <v>19</v>
       </c>
@@ -1613,68 +1607,67 @@
         <v>20</v>
       </c>
       <c r="L28" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="M28" t="s">
         <v>83</v>
       </c>
-      <c r="M28" t="s">
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="18">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" ht="15">
-      <c r="A29" s="20">
-        <v>18</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C29" s="18"/>
+      <c r="D29" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I29" s="5"/>
+      <c r="I29" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="14"/>
     </row>
-    <row r="30" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+    <row r="30" spans="1:15" ht="15" thickBot="1">
+      <c r="A30" s="19"/>
+      <c r="B30" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="14"/>
     </row>
-    <row r="31" spans="1:15" ht="15">
-      <c r="A31" s="20">
+    <row r="31" spans="1:15">
+      <c r="A31" s="18">
         <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="15" t="s">
-        <v>52</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="I31" s="5" t="s">
         <v>19</v>
       </c>
@@ -1682,53 +1675,44 @@
         <v>19</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L31" s="14"/>
       <c r="N31" t="s">
+        <v>88</v>
+      </c>
+      <c r="O31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="18"/>
+      <c r="B32" t="s">
         <v>89</v>
       </c>
-      <c r="O31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="15">
-      <c r="A32" s="20"/>
-      <c r="B32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" spans="1:13" ht="15">
-      <c r="A33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-    </row>
-    <row r="34" spans="1:13" ht="15">
-      <c r="A34" s="20"/>
-    </row>
-    <row r="35" spans="1:13" ht="15">
-      <c r="A35" s="20"/>
-    </row>
-    <row r="36" spans="1:13" ht="15">
-      <c r="A36" s="20"/>
-    </row>
-    <row r="39" spans="1:13" ht="15">
-      <c r="A39" s="20"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="18"/>
       <c r="M39" s="16"/>
     </row>
-    <row r="40" spans="1:13" ht="15">
-      <c r="A40" s="20"/>
+    <row r="40" spans="1:13">
+      <c r="A40" s="18"/>
       <c r="M40" s="16"/>
     </row>
   </sheetData>
@@ -1744,15 +1728,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010018AB406B7E83CB46A3914591FEF5E375" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="68b899bd1826a7b52dcc184dba4ca500">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b11c6198-3427-465c-8761-aa27f3e37317" xmlns:ns4="1bc7ac8e-978f-4930-988e-a7eebb614a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5996503ff4f0f28ffcbe3e2f7fae6153" ns3:_="" ns4:_="">
     <xsd:import namespace="b11c6198-3427-465c-8761-aa27f3e37317"/>
@@ -1961,20 +1936,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9413D6E-CC83-4DA9-B04D-98395BEF15B5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7949D86A-4ECE-4ACB-803E-DBA0DC1FCA2F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7949D86A-4ECE-4ACB-803E-DBA0DC1FCA2F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A004C57-C4A2-4105-A373-B1C1CD783209}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A004C57-C4A2-4105-A373-B1C1CD783209}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9413D6E-CC83-4DA9-B04D-98395BEF15B5}"/>
 </file>
</xml_diff>

<commit_message>
21 fertig, 18 weitergearbeitet
</commit_message>
<xml_diff>
--- a/feste-script/nublar_automation.xlsx
+++ b/feste-script/nublar_automation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://concat-my.sharepoint.com/personal/oliver_antwerpen_concat_de/Documents/Kunden/ITSG/DiGeN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{998A0B13-E7EC-481D-86CB-1CBB4CF5B6B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4440CD0F-E685-4AE2-95AA-5D545926D4BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6FC2A35C-60ED-4314-86AB-AEC6FD6F7C27}"/>
+    <workbookView xWindow="-25320" yWindow="1095" windowWidth="25440" windowHeight="15390" xr2:uid="{6FC2A35C-60ED-4314-86AB-AEC6FD6F7C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="92">
   <si>
     <t>#</t>
   </si>
@@ -198,7 +198,7 @@
     <t>Create Volume Template</t>
   </si>
   <si>
-    <t>OlAnt</t>
+    <t>X_20_createvolumetemplate.yml</t>
   </si>
   <si>
     <t>Create Volumes</t>
@@ -294,10 +294,16 @@
     <t>FeSte</t>
   </si>
   <si>
+    <t>X_18_addhypervisorclusterprofile.yml</t>
+  </si>
+  <si>
     <t>Add Hypervisors</t>
   </si>
   <si>
     <t>Create SP Template</t>
+  </si>
+  <si>
+    <t>X_17_createserverprofiletemplate.yml</t>
   </si>
   <si>
     <t>12,13,14</t>
@@ -430,12 +436,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -488,10 +493,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+  <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -808,7 +811,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1327,9 +1330,6 @@
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
-      <c r="H19" s="15" t="s">
-        <v>54</v>
-      </c>
       <c r="I19" s="5" t="s">
         <v>19</v>
       </c>
@@ -1339,7 +1339,9 @@
       <c r="K19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="14"/>
+      <c r="L19" s="14" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="18">
@@ -1355,15 +1357,18 @@
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
-      <c r="H20" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
+      <c r="I20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="L20" s="14"/>
     </row>
-    <row r="21" spans="1:15" ht="15">
+    <row r="21" spans="1:15">
       <c r="A21" s="18">
         <v>7</v>
       </c>
@@ -1392,7 +1397,7 @@
       <c r="M21" t="s">
         <v>58</v>
       </c>
-      <c r="O21" s="22" t="s">
+      <c r="O21" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1646,14 +1651,16 @@
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="14"/>
+      <c r="L29" s="14" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="30" spans="1:15" ht="15" thickBot="1">
       <c r="A30" s="19">
         <v>22</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19" t="s">
@@ -1675,7 +1682,7 @@
         <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="18" t="s">
@@ -1693,9 +1700,11 @@
       <c r="K31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="14"/>
+      <c r="L31" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="N31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="O31" t="s">
         <v>80</v>
@@ -1704,7 +1713,7 @@
     <row r="32" spans="1:15">
       <c r="A32" s="18"/>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>

</xml_diff>

<commit_message>
18 weitergearbeitet, it filter
</commit_message>
<xml_diff>
--- a/feste-script/nublar_automation.xlsx
+++ b/feste-script/nublar_automation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://concat-my.sharepoint.com/personal/oliver_antwerpen_concat_de/Documents/Kunden/ITSG/DiGeN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_13dd\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4440CD0F-E685-4AE2-95AA-5D545926D4BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3CB1823-9AE6-4703-BB8B-32C6E197A0AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="1095" windowWidth="25440" windowHeight="15390" xr2:uid="{6FC2A35C-60ED-4314-86AB-AEC6FD6F7C27}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="92">
   <si>
     <t>#</t>
   </si>
@@ -483,13 +483,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -811,7 +811,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -833,14 +833,14 @@
     <col min="15" max="15" width="58.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="18"/>
+    <row r="1" spans="1:15" ht="15">
+      <c r="A1" s="20"/>
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:15" ht="15">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -864,13 +864,13 @@
       <c r="H2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="20" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="15" t="s">
@@ -886,62 +886,62 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="18"/>
+    <row r="3" spans="1:15" ht="15">
+      <c r="A3" s="20"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="18"/>
+      <c r="C3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="20"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="18"/>
+    <row r="4" spans="1:15" ht="15">
+      <c r="A4" s="20"/>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
+      <c r="C4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
       <c r="L4" s="14"/>
     </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="18">
+    <row r="5" spans="1:15" ht="15">
+      <c r="A5" s="20">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="18"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="20"/>
       <c r="I5" s="5" t="s">
         <v>19</v>
       </c>
@@ -958,20 +958,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1">
-      <c r="A6" s="18">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A6" s="20">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
       <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
@@ -988,7 +988,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" ht="15">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="15">
       <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>30</v>
@@ -1043,7 +1043,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="14"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" ht="15">
       <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
         <v>31</v>
@@ -1061,7 +1061,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" ht="15">
       <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
         <v>32</v>
@@ -1079,7 +1079,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="14"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" ht="15">
       <c r="A11" s="7"/>
       <c r="B11" s="2" t="s">
         <v>33</v>
@@ -1097,7 +1097,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="14"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" ht="15">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
         <v>34</v>
@@ -1119,7 +1119,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="14"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" ht="15">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" ht="15">
       <c r="A14" s="7">
         <v>2</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1">
+    <row r="15" spans="1:15" ht="15.75" thickBot="1">
       <c r="A15" s="8">
         <v>4</v>
       </c>
@@ -1226,20 +1226,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="18">
+    <row r="16" spans="1:15" ht="15">
+      <c r="A16" s="20">
         <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
       <c r="I16" s="5" t="s">
         <v>19</v>
       </c>
@@ -1256,20 +1256,20 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="18">
+    <row r="17" spans="1:15" ht="15">
+      <c r="A17" s="20">
         <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
       <c r="I17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1286,29 +1286,27 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="18">
+    <row r="18" spans="1:15" ht="15">
+      <c r="A18" s="20">
         <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
       <c r="I18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K18" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="K18" s="5"/>
       <c r="L18" s="14" t="s">
         <v>51</v>
       </c>
@@ -1316,72 +1314,68 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="18">
+    <row r="19" spans="1:15" ht="15">
+      <c r="A19" s="20">
         <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
       <c r="I19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K19" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="K19" s="5"/>
       <c r="L19" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="18">
+    <row r="20" spans="1:15" ht="15">
+      <c r="A20" s="20">
         <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
       <c r="I20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K20" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="K20" s="5"/>
       <c r="L20" s="14"/>
     </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="18">
+    <row r="21" spans="1:15" ht="15">
+      <c r="A21" s="20">
         <v>7</v>
       </c>
       <c r="B21" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
       <c r="I21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1401,20 +1395,20 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
-      <c r="A22" s="18">
+    <row r="22" spans="1:15" ht="15">
+      <c r="A22" s="20">
         <v>8</v>
       </c>
       <c r="B22" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
       <c r="I22" s="5" t="s">
         <v>19</v>
       </c>
@@ -1431,20 +1425,20 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="18">
+    <row r="23" spans="1:15" ht="15">
+      <c r="A23" s="20">
         <v>9</v>
       </c>
       <c r="B23" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
       <c r="I23" s="5" t="s">
         <v>19</v>
       </c>
@@ -1461,20 +1455,20 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="18">
+    <row r="24" spans="1:15" ht="15">
+      <c r="A24" s="20">
         <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
       <c r="I24" s="5" t="s">
         <v>19</v>
       </c>
@@ -1491,20 +1485,20 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="18">
+    <row r="25" spans="1:15" ht="15">
+      <c r="A25" s="20">
         <v>13</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
       <c r="I25" s="5" t="s">
         <v>19</v>
       </c>
@@ -1527,20 +1521,20 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="18">
+    <row r="26" spans="1:15" ht="15">
+      <c r="A26" s="20">
         <v>14</v>
       </c>
       <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
       <c r="I26" s="5" t="s">
         <v>19</v>
       </c>
@@ -1563,20 +1557,20 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15" thickBot="1">
-      <c r="A27" s="19">
+    <row r="27" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A27" s="18">
         <v>15</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
       <c r="I27" s="5" t="s">
         <v>19</v>
       </c>
@@ -1599,20 +1593,20 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="18">
+    <row r="28" spans="1:15" ht="15">
+      <c r="A28" s="20">
         <v>3</v>
       </c>
       <c r="B28" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
       <c r="I28" s="5" t="s">
         <v>19</v>
       </c>
@@ -1629,20 +1623,20 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="18">
+    <row r="29" spans="1:15" ht="15">
+      <c r="A29" s="20">
         <v>18</v>
       </c>
       <c r="B29" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="15" t="s">
         <v>85</v>
       </c>
@@ -1655,20 +1649,20 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15" thickBot="1">
-      <c r="A30" s="19">
+    <row r="30" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A30" s="18">
         <v>22</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="15" t="s">
         <v>20</v>
       </c>
@@ -1677,20 +1671,20 @@
       <c r="K30" s="5"/>
       <c r="L30" s="14"/>
     </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="18">
+    <row r="31" spans="1:15" ht="15">
+      <c r="A31" s="20">
         <v>17</v>
       </c>
       <c r="B31" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
       <c r="I31" s="5" t="s">
         <v>19</v>
       </c>
@@ -1710,34 +1704,34 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="18"/>
+    <row r="32" spans="1:15" ht="15">
+      <c r="A32" s="20"/>
       <c r="B32" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="18"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+    </row>
+    <row r="33" spans="1:13" ht="15">
+      <c r="A33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+    </row>
+    <row r="39" spans="1:13" ht="15">
+      <c r="A39" s="20"/>
       <c r="M39" s="16"/>
     </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="18"/>
+    <row r="40" spans="1:13" ht="15">
+      <c r="A40" s="20"/>
       <c r="M40" s="16"/>
     </row>
   </sheetData>
@@ -1753,6 +1747,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010018AB406B7E83CB46A3914591FEF5E375" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="68b899bd1826a7b52dcc184dba4ca500">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b11c6198-3427-465c-8761-aa27f3e37317" xmlns:ns4="1bc7ac8e-978f-4930-988e-a7eebb614a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5996503ff4f0f28ffcbe3e2f7fae6153" ns3:_="" ns4:_="">
     <xsd:import namespace="b11c6198-3427-465c-8761-aa27f3e37317"/>
@@ -1961,12 +1961,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1977,11 +1971,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7949D86A-4ECE-4ACB-803E-DBA0DC1FCA2F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A004C57-C4A2-4105-A373-B1C1CD783209}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A004C57-C4A2-4105-A373-B1C1CD783209}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7949D86A-4ECE-4ACB-803E-DBA0DC1FCA2F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>